<commit_message>
added auxiliary meta data
</commit_message>
<xml_diff>
--- a/data/OM23_field_data.xlsx
+++ b/data/OM23_field_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/trca9794_colorado_edu/Documents/projects/OM23/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tacaro/Documents/GitHub/Oman-2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{5AC0783B-E8CE-404C-8CC6-223C2C7862EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{399FF1A7-162F-234E-B7B2-199824D55EEE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB32309D-F776-F34F-98A5-B8956A1BEC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{F38D1B93-C875-2145-92BF-EB96D71FDAEA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F38D1B93-C875-2145-92BF-EB96D71FDAEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>well</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>BA4A-150</t>
+  </si>
+  <si>
+    <t>depth to water table (m)</t>
   </si>
 </sst>
 </file>
@@ -487,19 +490,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FA7F7A-9DF1-3848-8F17-C3066E245E62}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="233" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -527,8 +531,11 @@
       <c r="I1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -556,8 +563,11 @@
       <c r="I2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -585,8 +595,11 @@
       <c r="I3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -614,8 +627,11 @@
       <c r="I4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -643,8 +659,11 @@
       <c r="I5">
         <v>-297</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -672,8 +691,11 @@
       <c r="I6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -701,8 +723,11 @@
       <c r="I7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -730,8 +755,11 @@
       <c r="I8">
         <v>-404</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -759,8 +787,11 @@
       <c r="I9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -788,8 +819,11 @@
       <c r="I10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -817,8 +851,11 @@
       <c r="I11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -846,8 +883,11 @@
       <c r="I12">
         <v>-402</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -875,8 +915,11 @@
       <c r="I13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -903,6 +946,9 @@
       </c>
       <c r="I14" t="s">
         <v>19</v>
+      </c>
+      <c r="J14">
+        <v>13.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>